<commit_message>
Save increment of work for CreateTimeSeriesEventTable - mostly functional now and ready to test with graphing.
git-svn-id: file:///cygdrive/C/owf-svnrepos/TSTool-test/java_142/trunk@916 fa08ced2-b08f-4ccc-859c-2e92e4a1381a
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/CreateTimeSeriesEventTable/Data/SouthPlatte-WaterEvents.xlsx
+++ b/test/regression/commands/general/CreateTimeSeriesEventTable/Data/SouthPlatte-WaterEvents.xlsx
@@ -16,7 +16,7 @@
     <sheet name="EventTypes" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -122,6 +122,270 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify the State abbreviation only if event is statewide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify region name only if event is region-wide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify basin name only if event is basin-wide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify county name only if event is county-wide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify division only if event is division-wide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify district only if event is district-wide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify locale name only if event is local-wide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify site identifier only if event is specific to a site.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not sure yet how to use this.  It is easier to use the other columns to match events.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not sure yet how to use this.  It is easier to use the other columns to match events.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steve Malers:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+WKT = Well known text spatial shape.  Not sure yet how to use this.  It is easier to use the other columns to match events.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G16" authorId="0" shapeId="0">
       <text>
         <r>
@@ -175,7 +439,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="226">
   <si>
     <t>EventType</t>
   </si>
@@ -925,6 +1189,15 @@
   </si>
   <si>
     <t>EventEnd</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -1363,10 +1636,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,9 +1655,13 @@
     <col min="7" max="8" width="18.28515625" style="6" customWidth="1"/>
     <col min="9" max="9" width="31.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1414,22 +1693,37 @@
         <v>12</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1451,11 +1745,11 @@
       <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -1483,11 +1777,14 @@
       <c r="I3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>216</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1513,10 +1810,10 @@
         <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1541,11 +1838,14 @@
       <c r="I5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>216</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -1571,10 +1871,10 @@
         <v>7</v>
       </c>
       <c r="J6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>175</v>
       </c>
@@ -1599,11 +1899,14 @@
       <c r="I7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>216</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -1626,10 +1929,10 @@
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>93</v>
       </c>
@@ -1655,10 +1958,10 @@
         <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -1683,11 +1986,14 @@
       <c r="I10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>216</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1713,10 +2019,10 @@
         <v>7</v>
       </c>
       <c r="J11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>103</v>
       </c>
@@ -1745,10 +2051,10 @@
         <v>7</v>
       </c>
       <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>192</v>
       </c>
@@ -1773,11 +2079,14 @@
       <c r="I13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>216</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1803,10 +2112,10 @@
         <v>7</v>
       </c>
       <c r="J14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1832,10 +2141,10 @@
         <v>7</v>
       </c>
       <c r="J15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1860,11 +2169,16 @@
       <c r="I16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1889,8 +2203,14 @@
       <c r="I17" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>223</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1916,10 +2236,10 @@
         <v>7</v>
       </c>
       <c r="J18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1945,10 +2265,10 @@
         <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1974,10 +2294,10 @@
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>65</v>
       </c>
@@ -2004,10 +2324,10 @@
         <v>7</v>
       </c>
       <c r="J21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>67</v>
       </c>
@@ -2033,10 +2353,10 @@
         <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -2061,11 +2381,14 @@
       <c r="I23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>216</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2090,11 +2413,14 @@
       <c r="I24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>216</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>68</v>
       </c>
@@ -2120,10 +2446,10 @@
         <v>7</v>
       </c>
       <c r="J25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2150,10 +2476,10 @@
         <v>7</v>
       </c>
       <c r="J26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2179,10 +2505,10 @@
         <v>7</v>
       </c>
       <c r="J27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2208,10 +2534,10 @@
         <v>7</v>
       </c>
       <c r="J28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>200</v>
       </c>
@@ -2237,10 +2563,10 @@
         <v>7</v>
       </c>
       <c r="J29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -2269,10 +2595,10 @@
         <v>7</v>
       </c>
       <c r="J30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -2297,11 +2623,14 @@
       <c r="I31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>223</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -2327,10 +2656,10 @@
         <v>7</v>
       </c>
       <c r="J32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -2356,10 +2685,10 @@
         <v>7</v>
       </c>
       <c r="J33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -2388,10 +2717,10 @@
         <v>7</v>
       </c>
       <c r="J34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -2417,11 +2746,14 @@
       <c r="I35" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>216</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -2446,11 +2778,14 @@
       <c r="I36" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>216</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -2476,10 +2811,10 @@
         <v>7</v>
       </c>
       <c r="J37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -2504,11 +2839,14 @@
       <c r="I38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>216</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -2536,11 +2874,14 @@
       <c r="I39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>216</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -2565,11 +2906,14 @@
       <c r="I40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>216</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -2594,11 +2938,14 @@
       <c r="I41" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>216</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -2623,11 +2970,14 @@
       <c r="I42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>216</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -2652,8 +3002,14 @@
       <c r="I43" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>216</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2678,11 +3034,14 @@
       <c r="I44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>216</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>131</v>
       </c>
@@ -2711,10 +3070,10 @@
         <v>7</v>
       </c>
       <c r="J45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -2742,11 +3101,14 @@
       <c r="I46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>216</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -2774,11 +3136,14 @@
       <c r="I47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>216</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -2803,11 +3168,14 @@
       <c r="I48" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J48" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L48" t="s">
+        <v>216</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>142</v>
       </c>
@@ -2832,11 +3200,11 @@
       <c r="I49" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="J49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K49" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>145</v>
       </c>
@@ -2862,10 +3230,10 @@
         <v>7</v>
       </c>
       <c r="J50" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -2891,10 +3259,10 @@
         <v>7</v>
       </c>
       <c r="J51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>152</v>
       </c>
@@ -2923,10 +3291,10 @@
         <v>7</v>
       </c>
       <c r="J52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>153</v>
       </c>
@@ -2953,10 +3321,10 @@
         <v>7</v>
       </c>
       <c r="J53" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>158</v>
       </c>
@@ -2984,11 +3352,11 @@
       <c r="I54" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="J54" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -3016,11 +3384,14 @@
       <c r="I55" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J55" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="L55" t="s">
+        <v>216</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>162</v>
       </c>
@@ -3046,7 +3417,7 @@
         <v>7</v>
       </c>
       <c r="J56" t="s">
-        <v>7</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tests that were omitted from original SVN to Git migration because of a slight gap in time between last SVN commit and local work.
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/CreateTimeSeriesEventTable/Data/SouthPlatte-WaterEvents.xlsx
+++ b/test/regression/commands/general/CreateTimeSeriesEventTable/Data/SouthPlatte-WaterEvents.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EventData" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -439,7 +440,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="252">
   <si>
     <t>EventType</t>
   </si>
@@ -1198,6 +1199,84 @@
   </si>
   <si>
     <t>Site</t>
+  </si>
+  <si>
+    <t>IconOriginalName</t>
+  </si>
+  <si>
+    <t>cloud_rain_icon.png</t>
+  </si>
+  <si>
+    <t>water_sea.png</t>
+  </si>
+  <si>
+    <t>sun.png</t>
+  </si>
+  <si>
+    <t>document_text_edit_32.png</t>
+  </si>
+  <si>
+    <t>document_text_add_32.png</t>
+  </si>
+  <si>
+    <t>blur_gear.png</t>
+  </si>
+  <si>
+    <t>snow_flake.png</t>
+  </si>
+  <si>
+    <t>group_half_32.png</t>
+  </si>
+  <si>
+    <t>oilwell.png</t>
+  </si>
+  <si>
+    <t>document_text_information_32.png</t>
+  </si>
+  <si>
+    <t>Basic-Scales-of-Balance-icon.png</t>
+  </si>
+  <si>
+    <t>chat_exclamation.png</t>
+  </si>
+  <si>
+    <t>ColoradoLawCourtCase.png</t>
+  </si>
+  <si>
+    <t>IconName</t>
+  </si>
+  <si>
+    <t>ColoradoLawImplemented.png</t>
+  </si>
+  <si>
+    <t>ColoradoLawPassed.png</t>
+  </si>
+  <si>
+    <t>Drought.png</t>
+  </si>
+  <si>
+    <t>Flood.png</t>
+  </si>
+  <si>
+    <t>HighGroundWaterReports.png</t>
+  </si>
+  <si>
+    <t>Snowpack.png</t>
+  </si>
+  <si>
+    <t>Study.png</t>
+  </si>
+  <si>
+    <t>Technology.png</t>
+  </si>
+  <si>
+    <t>WellAugmentationGroup.png</t>
+  </si>
+  <si>
+    <t>WellConstruction.png</t>
+  </si>
+  <si>
+    <t>WetYears.png</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
@@ -3446,120 +3525,200 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>148</v>
       </c>
       <c r="B8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
       <c r="B10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
       <c r="B11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D13" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>